<commit_message>
Criação Home Page Part-1
-Definicão do Template Bootstrap
-Definição dos Atributos da Nav Bar
</commit_message>
<xml_diff>
--- a/doc/Diarios/DiarioTabela.xlsx
+++ b/doc/Diarios/DiarioTabela.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Data</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>2h</t>
+  </si>
+  <si>
+    <t>Grupo 10</t>
+  </si>
+  <si>
+    <t>29/10/2017</t>
+  </si>
+  <si>
+    <t>Criação Home Page</t>
   </si>
 </sst>
 </file>
@@ -364,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:D6"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,6 +386,11 @@
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
@@ -413,6 +427,21 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="e">
+        <f>-Definicao do Template de todas as Páginas do Site, United Template     -Definicão dos Atributos da Página Home -Criação de algumas Views</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>